<commit_message>
Day 3 | DA 16
</commit_message>
<xml_diff>
--- a/Batch/16/Day_1.xlsx
+++ b/Batch/16/Day_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28829"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive\Work\Acciojob\Modules\statistics\Batch\16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCD1A83-F8D0-4F68-963F-196824E973DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45969C09-26F0-4510-BBFD-FB740363D209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="118">
   <si>
     <t>Large amount of data</t>
   </si>
@@ -374,6 +374,18 @@
   </si>
   <si>
     <t>There is some temp</t>
+  </si>
+  <si>
+    <t>Column Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>Scale Of Measurement</t>
   </si>
 </sst>
 </file>
@@ -650,29 +662,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -686,16 +677,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -713,19 +695,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -735,6 +708,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2061,8 +2073,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3740852" y="1624191"/>
-          <a:ext cx="635865" cy="302614"/>
+          <a:off x="3753268" y="1645543"/>
+          <a:ext cx="643928" cy="306451"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2076,13 +2088,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="206222"/>
+                <a:pt x="0" y="208837"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="635865" y="206222"/>
+                <a:pt x="643928" y="208837"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="635865" y="302614"/>
+                <a:pt x="643928" y="306451"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2123,8 +2135,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3104987" y="1624191"/>
-          <a:ext cx="635865" cy="302614"/>
+          <a:off x="3109340" y="1645543"/>
+          <a:ext cx="643928" cy="306451"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2135,16 +2147,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="635865" y="0"/>
+                <a:pt x="643928" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="635865" y="206222"/>
+                <a:pt x="643928" y="208837"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="206222"/>
+                <a:pt x="0" y="208837"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="302614"/>
+                <a:pt x="0" y="306451"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2185,8 +2197,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2469122" y="660855"/>
-          <a:ext cx="1271730" cy="302614"/>
+          <a:off x="2465412" y="669992"/>
+          <a:ext cx="1287856" cy="306451"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2200,13 +2212,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="206222"/>
+                <a:pt x="0" y="208837"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="1271730" y="206222"/>
+                <a:pt x="1287856" y="208837"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="1271730" y="302614"/>
+                <a:pt x="1287856" y="306451"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2247,8 +2259,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1197391" y="1624191"/>
-          <a:ext cx="635865" cy="302614"/>
+          <a:off x="1177556" y="1645543"/>
+          <a:ext cx="643928" cy="306451"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2262,13 +2274,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="206222"/>
+                <a:pt x="0" y="208837"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="635865" y="206222"/>
+                <a:pt x="643928" y="208837"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="635865" y="302614"/>
+                <a:pt x="643928" y="306451"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2309,8 +2321,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="561525" y="1624191"/>
-          <a:ext cx="635865" cy="302614"/>
+          <a:off x="533628" y="1645543"/>
+          <a:ext cx="643928" cy="306451"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2321,16 +2333,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="635865" y="0"/>
+                <a:pt x="643928" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="635865" y="206222"/>
+                <a:pt x="643928" y="208837"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="206222"/>
+                <a:pt x="0" y="208837"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="302614"/>
+                <a:pt x="0" y="306451"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2371,8 +2383,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1197391" y="660855"/>
-          <a:ext cx="1271730" cy="302614"/>
+          <a:off x="1177556" y="669992"/>
+          <a:ext cx="1287856" cy="306451"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2383,16 +2395,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="1271730" y="0"/>
+                <a:pt x="1287856" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="1271730" y="206222"/>
+                <a:pt x="1287856" y="208837"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="206222"/>
+                <a:pt x="0" y="208837"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="302614"/>
+                <a:pt x="0" y="306451"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2433,8 +2445,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1948868" y="133"/>
-          <a:ext cx="1040507" cy="660721"/>
+          <a:off x="1938562" y="892"/>
+          <a:ext cx="1053700" cy="669099"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -2485,8 +2497,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2064480" y="109964"/>
-          <a:ext cx="1040507" cy="660721"/>
+          <a:off x="2055640" y="112116"/>
+          <a:ext cx="1053700" cy="669099"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -2529,12 +2541,12 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="49530" tIns="49530" rIns="49530" bIns="49530" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="53340" tIns="53340" rIns="53340" bIns="53340" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="622300">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -2547,14 +2559,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-IN" sz="1300" kern="1200"/>
+            <a:rPr lang="en-IN" sz="1400" kern="1200"/>
             <a:t>Data</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2083832" y="129316"/>
-        <a:ext cx="1001803" cy="622017"/>
+        <a:off x="2075237" y="131713"/>
+        <a:ext cx="1014506" cy="629905"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{35615F8A-B830-4FD8-B5E7-4D6E19670810}">
@@ -2564,8 +2576,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="677137" y="963469"/>
-          <a:ext cx="1040507" cy="660721"/>
+          <a:off x="650706" y="976443"/>
+          <a:ext cx="1053700" cy="669099"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -2616,8 +2628,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="792749" y="1073300"/>
-          <a:ext cx="1040507" cy="660721"/>
+          <a:off x="767784" y="1087667"/>
+          <a:ext cx="1053700" cy="669099"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -2660,12 +2672,12 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="49530" tIns="49530" rIns="49530" bIns="49530" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="53340" tIns="53340" rIns="53340" bIns="53340" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="622300">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -2678,14 +2690,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-IN" sz="1300" kern="1200"/>
+            <a:rPr lang="en-IN" sz="1400" kern="1200"/>
             <a:t>Categorical / Quaitative</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="812101" y="1092652"/>
-        <a:ext cx="1001803" cy="622017"/>
+        <a:off x="787381" y="1107264"/>
+        <a:ext cx="1014506" cy="629905"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{B89F44F6-6A0A-4190-987D-EBD3E2D89792}">
@@ -2695,8 +2707,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="41272" y="1926805"/>
-          <a:ext cx="1040507" cy="660721"/>
+          <a:off x="6778" y="1951994"/>
+          <a:ext cx="1053700" cy="669099"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -2747,8 +2759,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="156884" y="2036636"/>
-          <a:ext cx="1040507" cy="660721"/>
+          <a:off x="123856" y="2063218"/>
+          <a:ext cx="1053700" cy="669099"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -2791,12 +2803,12 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="49530" tIns="49530" rIns="49530" bIns="49530" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="53340" tIns="53340" rIns="53340" bIns="53340" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="622300">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -2809,14 +2821,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-IN" sz="1300" kern="1200"/>
+            <a:rPr lang="en-IN" sz="1400" kern="1200"/>
             <a:t>Nominal</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="176236" y="2055988"/>
-        <a:ext cx="1001803" cy="622017"/>
+        <a:off x="143453" y="2082815"/>
+        <a:ext cx="1014506" cy="629905"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{AB88C2E0-85CC-4258-A873-500DE958F3A0}">
@@ -2826,8 +2838,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1313003" y="1926805"/>
-          <a:ext cx="1040507" cy="660721"/>
+          <a:off x="1294634" y="1951994"/>
+          <a:ext cx="1053700" cy="669099"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -2878,8 +2890,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1428615" y="2036636"/>
-          <a:ext cx="1040507" cy="660721"/>
+          <a:off x="1411712" y="2063218"/>
+          <a:ext cx="1053700" cy="669099"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -2922,12 +2934,12 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="49530" tIns="49530" rIns="49530" bIns="49530" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="53340" tIns="53340" rIns="53340" bIns="53340" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="622300">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -2940,14 +2952,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-IN" sz="1300" kern="1200"/>
+            <a:rPr lang="en-IN" sz="1400" kern="1200"/>
             <a:t>Ordinal</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1447967" y="2055988"/>
-        <a:ext cx="1001803" cy="622017"/>
+        <a:off x="1431309" y="2082815"/>
+        <a:ext cx="1014506" cy="629905"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{37BF41EB-566D-4264-BF21-648D7198B4BD}">
@@ -2957,8 +2969,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3220599" y="963469"/>
-          <a:ext cx="1040507" cy="660721"/>
+          <a:off x="3226418" y="976443"/>
+          <a:ext cx="1053700" cy="669099"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -3009,8 +3021,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3336211" y="1073300"/>
-          <a:ext cx="1040507" cy="660721"/>
+          <a:off x="3343496" y="1087667"/>
+          <a:ext cx="1053700" cy="669099"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -3053,12 +3065,12 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="49530" tIns="49530" rIns="49530" bIns="49530" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="53340" tIns="53340" rIns="53340" bIns="53340" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="622300">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3071,14 +3083,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-IN" sz="1300" kern="1200"/>
+            <a:rPr lang="en-IN" sz="1400" kern="1200"/>
             <a:t>Numerical / Quantitative</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3355563" y="1092652"/>
-        <a:ext cx="1001803" cy="622017"/>
+        <a:off x="3363093" y="1107264"/>
+        <a:ext cx="1014506" cy="629905"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{887AC4C3-8407-4569-9CD8-188E5BBC657D}">
@@ -3088,8 +3100,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2584733" y="1926805"/>
-          <a:ext cx="1040507" cy="660721"/>
+          <a:off x="2582490" y="1951994"/>
+          <a:ext cx="1053700" cy="669099"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -3140,8 +3152,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2700345" y="2036636"/>
-          <a:ext cx="1040507" cy="660721"/>
+          <a:off x="2699568" y="2063218"/>
+          <a:ext cx="1053700" cy="669099"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -3184,12 +3196,12 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="49530" tIns="49530" rIns="49530" bIns="49530" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="53340" tIns="53340" rIns="53340" bIns="53340" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="622300">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3202,14 +3214,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-IN" sz="1300" kern="1200"/>
+            <a:rPr lang="en-IN" sz="1400" kern="1200"/>
             <a:t>Discrete</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2719697" y="2055988"/>
-        <a:ext cx="1001803" cy="622017"/>
+        <a:off x="2719165" y="2082815"/>
+        <a:ext cx="1014506" cy="629905"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{96476A14-9539-4C25-AB88-D7F63B726A4F}">
@@ -3219,8 +3231,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3856464" y="1926805"/>
-          <a:ext cx="1040507" cy="660721"/>
+          <a:off x="3870346" y="1951994"/>
+          <a:ext cx="1053700" cy="669099"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -3271,8 +3283,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3972076" y="2036636"/>
-          <a:ext cx="1040507" cy="660721"/>
+          <a:off x="3987424" y="2063218"/>
+          <a:ext cx="1053700" cy="669099"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -3315,12 +3327,12 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="49530" tIns="49530" rIns="49530" bIns="49530" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="53340" tIns="53340" rIns="53340" bIns="53340" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="622300">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3333,14 +3345,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-IN" sz="1300" kern="1200"/>
+            <a:rPr lang="en-IN" sz="1400" kern="1200"/>
             <a:t>Continous</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3991428" y="2055988"/>
-        <a:ext cx="1001803" cy="622017"/>
+        <a:off x="4007021" y="2082815"/>
+        <a:ext cx="1014506" cy="629905"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -4980,8 +4992,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4638926" y="2876550"/>
-          <a:ext cx="5342541" cy="3790950"/>
+          <a:off x="4639486" y="2851337"/>
+          <a:ext cx="5344222" cy="3769098"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5299,8 +5311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G81"/>
   <sheetViews>
-    <sheetView topLeftCell="C55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66:G69"/>
+    <sheetView topLeftCell="B18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48:G81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="48.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5399,96 +5411,96 @@
       </c>
     </row>
     <row r="18" spans="5:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="28" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="19" spans="5:6" x14ac:dyDescent="0.45">
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
     </row>
     <row r="20" spans="5:6" x14ac:dyDescent="0.45">
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
     </row>
     <row r="21" spans="5:6" x14ac:dyDescent="0.45">
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
     </row>
     <row r="22" spans="5:6" x14ac:dyDescent="0.45">
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
     </row>
     <row r="23" spans="5:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
     </row>
     <row r="24" spans="5:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="28" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" spans="5:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
     </row>
     <row r="26" spans="5:6" x14ac:dyDescent="0.45">
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
     </row>
     <row r="27" spans="5:6" x14ac:dyDescent="0.45">
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
     </row>
     <row r="28" spans="5:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
     </row>
     <row r="29" spans="5:6" x14ac:dyDescent="0.45">
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="F29" s="28" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="30" spans="5:6" x14ac:dyDescent="0.45">
-      <c r="E30" s="7"/>
-      <c r="F30" s="9"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="31"/>
     </row>
     <row r="31" spans="5:6" x14ac:dyDescent="0.45">
-      <c r="E31" s="7"/>
-      <c r="F31" s="9"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="31"/>
     </row>
     <row r="32" spans="5:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="E32" s="8"/>
-      <c r="F32" s="10"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="32"/>
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="E33" s="6" t="s">
+      <c r="E33" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F33" s="28" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="34" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="E34" s="7"/>
-      <c r="F34" s="9"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="31"/>
     </row>
     <row r="35" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="E35" s="7"/>
-      <c r="F35" s="9"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="31"/>
     </row>
     <row r="36" spans="4:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="E36" s="8"/>
-      <c r="F36" s="10"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="32"/>
     </row>
     <row r="39" spans="4:7" ht="17.649999999999999" x14ac:dyDescent="0.45">
       <c r="D39" s="2" t="s">
@@ -5552,363 +5564,379 @@
     </row>
     <row r="47" spans="4:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="48" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D48" s="15" t="s">
+      <c r="D48" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E48" s="16" t="s">
+      <c r="E48" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F48" s="16" t="s">
+      <c r="F48" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G48" s="17" t="s">
+      <c r="G48" s="10" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="49" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D49" s="18" t="s">
+      <c r="D49" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="E49" s="13" t="s">
+      <c r="E49" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="F49" s="14" t="s">
+      <c r="F49" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G49" s="19" t="s">
+      <c r="G49" s="11" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="50" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D50" s="18"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="14" t="s">
+      <c r="D50" s="33"/>
+      <c r="E50" s="35"/>
+      <c r="F50" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G50" s="19" t="s">
+      <c r="G50" s="11" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="51" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D51" s="18"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="14" t="s">
+      <c r="D51" s="33"/>
+      <c r="E51" s="35"/>
+      <c r="F51" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G51" s="19" t="s">
+      <c r="G51" s="11" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="52" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D52" s="18"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="14" t="s">
+      <c r="D52" s="33"/>
+      <c r="E52" s="35"/>
+      <c r="F52" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G52" s="19"/>
+      <c r="G52" s="11"/>
     </row>
     <row r="53" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D53" s="18"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="14" t="s">
+      <c r="D53" s="33"/>
+      <c r="E53" s="35"/>
+      <c r="F53" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G53" s="19"/>
+      <c r="G53" s="11"/>
     </row>
     <row r="54" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D54" s="18" t="s">
+      <c r="D54" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="E54" s="13" t="s">
+      <c r="E54" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="F54" s="14" t="s">
+      <c r="F54" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G54" s="19" t="s">
+      <c r="G54" s="11" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="55" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D55" s="18"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="14" t="s">
+      <c r="D55" s="33"/>
+      <c r="E55" s="35"/>
+      <c r="F55" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G55" s="19" t="s">
+      <c r="G55" s="11" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="56" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D56" s="18"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="14" t="s">
+      <c r="D56" s="33"/>
+      <c r="E56" s="35"/>
+      <c r="F56" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G56" s="19" t="s">
+      <c r="G56" s="11" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="57" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D57" s="18"/>
-      <c r="E57" s="13"/>
-      <c r="F57" s="14" t="s">
+      <c r="D57" s="33"/>
+      <c r="E57" s="35"/>
+      <c r="F57" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="G57" s="19"/>
+      <c r="G57" s="11"/>
     </row>
     <row r="58" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D58" s="18" t="s">
+      <c r="D58" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="E58" s="13" t="s">
+      <c r="E58" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="F58" s="14" t="s">
+      <c r="F58" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="G58" s="19" t="s">
+      <c r="G58" s="11" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="59" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D59" s="18"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="14" t="s">
+      <c r="D59" s="33"/>
+      <c r="E59" s="35"/>
+      <c r="F59" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="G59" s="19" t="s">
+      <c r="G59" s="11" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="60" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D60" s="18"/>
-      <c r="E60" s="13"/>
-      <c r="F60" s="14" t="s">
+      <c r="D60" s="33"/>
+      <c r="E60" s="35"/>
+      <c r="F60" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="G60" s="19" t="s">
+      <c r="G60" s="11" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="61" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D61" s="18" t="s">
+      <c r="D61" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="E61" s="13" t="s">
+      <c r="E61" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="F61" s="14" t="s">
+      <c r="F61" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="G61" s="19" t="s">
+      <c r="G61" s="11" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="62" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D62" s="18"/>
-      <c r="E62" s="13"/>
-      <c r="F62" s="14" t="s">
+      <c r="D62" s="33"/>
+      <c r="E62" s="35"/>
+      <c r="F62" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="G62" s="19" t="s">
+      <c r="G62" s="11" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="63" spans="4:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D63" s="20"/>
-      <c r="E63" s="21"/>
-      <c r="F63" s="22" t="s">
+      <c r="D63" s="34"/>
+      <c r="E63" s="36"/>
+      <c r="F63" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="G63" s="23" t="s">
+      <c r="G63" s="13" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="64" spans="4:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="E64" s="34"/>
-      <c r="F64" s="34"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="21"/>
     </row>
     <row r="65" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D65" s="24" t="s">
+      <c r="D65" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E65" s="25" t="s">
+      <c r="E65" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F65" s="25" t="s">
+      <c r="F65" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="G65" s="26" t="s">
+      <c r="G65" s="16" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="66" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D66" s="27" t="s">
+      <c r="D66" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E66" s="11" t="s">
+      <c r="E66" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="F66" s="12" t="s">
+      <c r="F66" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="G66" s="28" t="s">
+      <c r="G66" s="17" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="67" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D67" s="27"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="12" t="s">
+      <c r="D67" s="24"/>
+      <c r="E67" s="26"/>
+      <c r="F67" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="G67" s="28" t="s">
+      <c r="G67" s="17" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="68" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D68" s="27"/>
-      <c r="E68" s="11"/>
-      <c r="F68" s="12" t="s">
+      <c r="D68" s="24"/>
+      <c r="E68" s="26"/>
+      <c r="F68" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="G68" s="28" t="s">
+      <c r="G68" s="17" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="69" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D69" s="27"/>
-      <c r="E69" s="11"/>
-      <c r="F69" s="12" t="s">
+      <c r="D69" s="24"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="G69" s="28"/>
+      <c r="G69" s="17"/>
     </row>
     <row r="70" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D70" s="27" t="s">
+      <c r="D70" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="11" t="s">
+      <c r="E70" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="F70" s="12" t="s">
+      <c r="F70" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="G70" s="28" t="s">
+      <c r="G70" s="17" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="71" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D71" s="27"/>
-      <c r="E71" s="11"/>
-      <c r="F71" s="12" t="s">
+      <c r="D71" s="24"/>
+      <c r="E71" s="26"/>
+      <c r="F71" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="G71" s="28" t="s">
+      <c r="G71" s="17" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="72" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D72" s="27"/>
-      <c r="E72" s="11"/>
-      <c r="F72" s="12" t="s">
+      <c r="D72" s="24"/>
+      <c r="E72" s="26"/>
+      <c r="F72" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G72" s="28" t="s">
+      <c r="G72" s="17" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="73" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D73" s="27"/>
-      <c r="E73" s="11"/>
-      <c r="F73" s="12" t="s">
+      <c r="D73" s="24"/>
+      <c r="E73" s="26"/>
+      <c r="F73" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="G73" s="28"/>
+      <c r="G73" s="17"/>
     </row>
     <row r="74" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D74" s="27" t="s">
+      <c r="D74" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="E74" s="11" t="s">
+      <c r="E74" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="F74" s="12" t="s">
+      <c r="F74" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G74" s="28" t="s">
+      <c r="G74" s="17" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="75" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D75" s="27"/>
-      <c r="E75" s="11"/>
-      <c r="F75" s="12" t="s">
+      <c r="D75" s="24"/>
+      <c r="E75" s="26"/>
+      <c r="F75" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="G75" s="28" t="s">
+      <c r="G75" s="17" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="76" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D76" s="27"/>
-      <c r="E76" s="11"/>
-      <c r="F76" s="12" t="s">
+      <c r="D76" s="24"/>
+      <c r="E76" s="26"/>
+      <c r="F76" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="G76" s="28" t="s">
+      <c r="G76" s="17" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="77" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D77" s="27"/>
-      <c r="E77" s="11"/>
-      <c r="F77" s="12" t="s">
+      <c r="D77" s="24"/>
+      <c r="E77" s="26"/>
+      <c r="F77" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="G77" s="28" t="s">
+      <c r="G77" s="17" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="78" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D78" s="27" t="s">
+      <c r="D78" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="E78" s="11" t="s">
+      <c r="E78" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="F78" s="12" t="s">
+      <c r="F78" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="G78" s="29"/>
+      <c r="G78" s="18"/>
     </row>
     <row r="79" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D79" s="27"/>
-      <c r="E79" s="11"/>
-      <c r="F79" s="12" t="s">
+      <c r="D79" s="24"/>
+      <c r="E79" s="26"/>
+      <c r="F79" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="G79" s="29"/>
+      <c r="G79" s="18"/>
     </row>
     <row r="80" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D80" s="27"/>
-      <c r="E80" s="11"/>
-      <c r="F80" s="12" t="s">
+      <c r="D80" s="24"/>
+      <c r="E80" s="26"/>
+      <c r="F80" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="G80" s="29"/>
+      <c r="G80" s="18"/>
     </row>
     <row r="81" spans="4:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D81" s="30"/>
-      <c r="E81" s="31"/>
-      <c r="F81" s="32" t="s">
+      <c r="D81" s="25"/>
+      <c r="E81" s="27"/>
+      <c r="F81" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="G81" s="33"/>
+      <c r="G81" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="D61:D63"/>
+    <mergeCell ref="E61:E63"/>
+    <mergeCell ref="D49:D53"/>
+    <mergeCell ref="E49:E53"/>
+    <mergeCell ref="D54:D57"/>
+    <mergeCell ref="E54:E57"/>
+    <mergeCell ref="D58:D60"/>
+    <mergeCell ref="E58:E60"/>
+    <mergeCell ref="E33:E36"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="F33:F36"/>
+    <mergeCell ref="E18:E23"/>
+    <mergeCell ref="F18:F23"/>
+    <mergeCell ref="E24:E28"/>
+    <mergeCell ref="F24:F28"/>
     <mergeCell ref="D78:D81"/>
     <mergeCell ref="E78:E81"/>
     <mergeCell ref="D66:D69"/>
@@ -5917,22 +5945,6 @@
     <mergeCell ref="E70:E73"/>
     <mergeCell ref="D74:D77"/>
     <mergeCell ref="E74:E77"/>
-    <mergeCell ref="E33:E36"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="F29:F32"/>
-    <mergeCell ref="F33:F36"/>
-    <mergeCell ref="E18:E23"/>
-    <mergeCell ref="F18:F23"/>
-    <mergeCell ref="E24:E28"/>
-    <mergeCell ref="F24:F28"/>
-    <mergeCell ref="D61:D63"/>
-    <mergeCell ref="E61:E63"/>
-    <mergeCell ref="D49:D53"/>
-    <mergeCell ref="E49:E53"/>
-    <mergeCell ref="D54:D57"/>
-    <mergeCell ref="E54:E57"/>
-    <mergeCell ref="D58:D60"/>
-    <mergeCell ref="E58:E60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -5942,10 +5954,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C7F1E73-187C-4F33-ACA6-622528C944A1}">
-  <dimension ref="F18:P32"/>
+  <dimension ref="F18:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5954,21 +5966,21 @@
   </cols>
   <sheetData>
     <row r="18" spans="6:16" x14ac:dyDescent="0.45">
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
     </row>
     <row r="22" spans="6:16" x14ac:dyDescent="0.45">
-      <c r="I22" s="35"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35"/>
-      <c r="N22" s="35"/>
-      <c r="O22" s="35"/>
+      <c r="I22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="22"/>
     </row>
     <row r="25" spans="6:16" x14ac:dyDescent="0.45">
       <c r="I25" t="s">
@@ -6012,8 +6024,22 @@
       </c>
     </row>
     <row r="32" spans="6:16" x14ac:dyDescent="0.45">
-      <c r="F32" s="36">
+      <c r="F32" s="23">
         <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="6:9" x14ac:dyDescent="0.45">
+      <c r="F35" t="s">
+        <v>114</v>
+      </c>
+      <c r="G35" t="s">
+        <v>115</v>
+      </c>
+      <c r="H35" t="s">
+        <v>116</v>
+      </c>
+      <c r="I35" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>